<commit_message>
Dodavanje scenarija za prijavu i registraciju korisnika
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/PrijavaKorisnika.xlsx
+++ b/UseCaseIScenarij/PrijavaKorisnika.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>SCENARIJ:</t>
   </si>
@@ -40,12 +40,30 @@
     <t>Korisnik unosi tačne pristupne podatke</t>
   </si>
   <si>
-    <t>Posljedice:</t>
+    <t>Posljedice-uspješan završetak:</t>
   </si>
   <si>
     <t>Korisnik se prijavljuje i pristupa aplikaciji</t>
   </si>
   <si>
+    <t>Posljedice.neuspješan završetak:</t>
+  </si>
+  <si>
+    <t>Netačni pristupni podaci korisnika</t>
+  </si>
+  <si>
+    <t>Glavni akteri:</t>
+  </si>
+  <si>
+    <t>Korisnik</t>
+  </si>
+  <si>
+    <t>Ostali akteri:</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOK DOGAĐAJA: </t>
   </si>
   <si>
@@ -85,7 +103,16 @@
     <t>Korisnik unosi potrebne podatke i registruje se na aplikaciju</t>
   </si>
   <si>
+    <t>Unos svih potrebnih informacija i postojeće email adrese</t>
+  </si>
+  <si>
     <t>Uspješno registrovan korisnik na aplikaciju</t>
+  </si>
+  <si>
+    <t>Posljedice-neuspješan završetak:</t>
+  </si>
+  <si>
+    <t>Nepostojeća email adresa (nemogućnost verifikacije)</t>
   </si>
   <si>
     <t>TOK DOGAĐAJA:</t>
@@ -176,7 +203,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.0"/>
+    <col customWidth="1" min="1" max="1" width="28.14"/>
     <col customWidth="1" min="2" max="2" width="58.71"/>
   </cols>
   <sheetData>
@@ -225,110 +252,160 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="8">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
+      <c r="A11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>13</v>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>